<commit_message>
re-write json config, copy xlsx config, re-structure DatabaseExtract.py
</commit_message>
<xml_diff>
--- a/nifi/application/config/xlsx_config/IMMO_ES_CONFIG.xlsx
+++ b/nifi/application/config/xlsx_config/IMMO_ES_CONFIG.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="IMMO_ES" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,10 +17,11 @@
     <sheet name="PISOS" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="VENTADEPISOS" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="YAENCONTRE" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Glossary of Expectations" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="INDOMIO" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Glossary of Expectations" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">'Glossary of Expectations'!$A$1:$H$42</definedName>
+    <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">'Glossary of Expectations'!$A$1:$H$42</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="202">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -1012,7 +1013,7 @@
   </sheetPr>
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -1839,6 +1840,53 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <tabColor rgb="FF7030A0"/>
@@ -3570,16 +3618,16 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E22" type="list">
-      <formula1>'Glossary of Expectations'!$AB$2:$AB$11</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A20:A22" type="list">
+      <formula1>'Glossary of Expectations'!$C$2:$C$70</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F2:F22" type="list">
       <formula1>'Glossary of Expectations'!$AC$2:$AC$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A20:A22" type="list">
-      <formula1>'Glossary of Expectations'!$C$2:$C$70</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E22" type="list">
+      <formula1>'Glossary of Expectations'!$AB$2:$AB$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -3915,7 +3963,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>